<commit_message>
Set up example with global constraint
</commit_message>
<xml_diff>
--- a/test/example_biomass_synfuels_carbon_management_case.xlsx
+++ b/test/example_biomass_synfuels_carbon_management_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540F2249-59C9-7B40-BA29-B24DA9168D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DD680D-5128-ED47-B1D8-A2AA4EBBA0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="35420" windowHeight="21400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -341,10 +341,37 @@
     <t>OPTIONAL KEYWORDS, examples</t>
   </si>
   <si>
-    <t>p_max_pu</t>
-  </si>
-  <si>
     <t>Note: p_nom, p_min_pu and p_max_pu will be interpreted as e_* for Store components</t>
+  </si>
+  <si>
+    <t>GlobalConstraint</t>
+  </si>
+  <si>
+    <t>co2_limit</t>
+  </si>
+  <si>
+    <t>sense</t>
+  </si>
+  <si>
+    <t>carrier_attribute</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>co2_emissions</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>co2</t>
+  </si>
+  <si>
+    <t>carrier</t>
   </si>
 </sst>
 </file>
@@ -1233,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R73"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1555,7 +1582,7 @@
       </c>
       <c r="C32" s="8"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1567,7 +1594,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -1576,11 +1603,11 @@
         <v>9.9999999999417923</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1589,7 +1616,7 @@
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1601,7 +1628,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1613,11 +1640,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1626,7 +1653,7 @@
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1635,7 +1662,7 @@
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1644,14 +1671,14 @@
       </c>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="F43" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1659,7 +1686,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
         <v>46</v>
       </c>
@@ -1670,17 +1697,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>9</v>
       </c>
@@ -1688,25 +1720,25 @@
         <v>10</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>86</v>
@@ -1729,47 +1761,59 @@
       <c r="Q49" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>11</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>1</v>
       </c>
       <c r="L50" s="5"/>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B51" t="s">
         <v>74</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>74</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>1</v>
       </c>
       <c r="L51" s="5"/>
       <c r="O51" s="5"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>75</v>
       </c>
       <c r="K52">
@@ -1781,14 +1825,14 @@
       </c>
       <c r="O52" s="5"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>76</v>
       </c>
       <c r="K53">
@@ -1799,21 +1843,18 @@
         <v>1</v>
       </c>
       <c r="O53" s="5"/>
-      <c r="R53" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>11</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>76</v>
       </c>
       <c r="K54">
@@ -1824,20 +1865,20 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>77</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>76</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>75</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>79</v>
       </c>
       <c r="K55">
@@ -1851,36 +1892,33 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
-      </c>
-      <c r="C56" t="s">
-        <v>81</v>
-      </c>
-      <c r="H56">
-        <v>-1</v>
-      </c>
-      <c r="K56">
-        <v>1000</v>
+        <v>111</v>
       </c>
       <c r="L56" s="5"/>
       <c r="O56" s="5"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="U56">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
-      </c>
-      <c r="H57">
+        <v>111</v>
+      </c>
+      <c r="D57" t="s">
+        <v>81</v>
+      </c>
+      <c r="I57">
         <v>-1</v>
       </c>
       <c r="K57">
@@ -1889,299 +1927,337 @@
       <c r="L57" s="5"/>
       <c r="O57" s="5"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="D58" t="s">
         <v>79</v>
       </c>
-      <c r="E58" t="s">
-        <v>81</v>
+      <c r="I58">
+        <v>-1</v>
       </c>
       <c r="K58">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="L58" s="5"/>
-      <c r="O58" s="5">
-        <v>1</v>
-      </c>
-      <c r="P58">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O58" s="5"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
-      </c>
-      <c r="C59" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="E59" t="s">
+        <v>79</v>
+      </c>
+      <c r="F59" t="s">
         <v>81</v>
       </c>
       <c r="K59">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L59" s="5"/>
       <c r="O59" s="5">
         <v>1</v>
       </c>
       <c r="P59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" t="s">
+        <v>81</v>
+      </c>
+      <c r="K60">
+        <v>2</v>
+      </c>
+      <c r="L60" s="5"/>
+      <c r="O60" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="P60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>85</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D61" t="s">
         <v>85</v>
       </c>
-      <c r="J60">
+      <c r="J61">
         <v>50</v>
       </c>
-      <c r="K60">
+      <c r="K61">
         <v>50</v>
       </c>
-      <c r="L60" s="5">
+      <c r="L61" s="5">
         <v>20</v>
       </c>
-      <c r="M60" t="str">
+      <c r="M61" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
-      <c r="O60" s="5"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B61" t="s">
-        <v>87</v>
-      </c>
-      <c r="C61" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>81</v>
-      </c>
-      <c r="L61" s="5"/>
-      <c r="O61" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="P61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O61" s="5"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" t="s">
         <v>85</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>79</v>
       </c>
       <c r="F62" t="s">
         <v>81</v>
       </c>
       <c r="L62" s="5"/>
       <c r="O62" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" t="s">
+        <v>85</v>
+      </c>
+      <c r="E63" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" t="s">
+        <v>79</v>
+      </c>
+      <c r="G63" t="s">
+        <v>81</v>
+      </c>
+      <c r="L63" s="5"/>
+      <c r="O63" s="5">
         <v>0.4</v>
       </c>
-      <c r="P62">
+      <c r="P63">
         <v>0.9</v>
       </c>
-      <c r="Q62">
+      <c r="Q63">
         <v>0.1</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>90</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D64" t="s">
         <v>90</v>
       </c>
-      <c r="J63">
+      <c r="J64">
         <v>40</v>
       </c>
-      <c r="K63">
+      <c r="K64">
         <v>40</v>
       </c>
-      <c r="L63" s="5">
+      <c r="L64" s="5">
         <v>20</v>
       </c>
-      <c r="M63" t="str">
+      <c r="M64" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B64" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" t="s">
-        <v>90</v>
-      </c>
-      <c r="D64" t="s">
-        <v>11</v>
-      </c>
-      <c r="L64" s="5"/>
-      <c r="O64" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
-      </c>
-      <c r="C65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" t="s">
         <v>90</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>11</v>
-      </c>
-      <c r="E65" t="s">
-        <v>79</v>
-      </c>
-      <c r="F65" t="s">
-        <v>81</v>
       </c>
       <c r="L65" s="5"/>
       <c r="O65" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B66" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" t="s">
+        <v>90</v>
+      </c>
+      <c r="E66" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" t="s">
+        <v>79</v>
+      </c>
+      <c r="G66" t="s">
+        <v>81</v>
+      </c>
+      <c r="L66" s="5"/>
+      <c r="O66" s="5">
         <v>0.4</v>
       </c>
-      <c r="P65">
+      <c r="P66">
         <v>1</v>
       </c>
-      <c r="Q65">
+      <c r="Q66">
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>93</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D67" t="s">
         <v>93</v>
       </c>
-      <c r="J66">
+      <c r="J67">
         <v>15</v>
       </c>
-      <c r="K66">
+      <c r="K67">
         <v>15</v>
       </c>
-      <c r="L66" s="5">
+      <c r="L67" s="5">
         <v>50</v>
       </c>
-      <c r="M66" t="str">
+      <c r="M67" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B67" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" t="s">
-        <v>93</v>
-      </c>
-      <c r="D67" t="s">
-        <v>11</v>
-      </c>
-      <c r="L67" s="5"/>
-      <c r="O67" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" t="s">
         <v>93</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>11</v>
-      </c>
-      <c r="E68" t="s">
-        <v>79</v>
-      </c>
-      <c r="F68" t="s">
-        <v>81</v>
       </c>
       <c r="L68" s="5"/>
       <c r="O68" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B69" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" t="s">
+        <v>93</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>79</v>
+      </c>
+      <c r="G69" t="s">
+        <v>81</v>
+      </c>
+      <c r="L69" s="5"/>
+      <c r="O69" s="5">
         <v>0.4</v>
       </c>
-      <c r="P68">
+      <c r="P69">
         <v>1</v>
       </c>
-      <c r="Q68">
+      <c r="Q69">
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70" t="s">
+        <v>104</v>
+      </c>
+      <c r="L70" s="5"/>
+      <c r="O70" s="5"/>
+      <c r="R70" t="s">
+        <v>108</v>
+      </c>
+      <c r="S70" t="s">
+        <v>109</v>
+      </c>
+      <c r="T70">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>51</v>
       </c>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>